<commit_message>
updated step definition file CreateContact
</commit_message>
<xml_diff>
--- a/FreeCrm/src/test/resources/CreateContactxlss/validData.xlsx
+++ b/FreeCrm/src/test/resources/CreateContactxlss/validData.xlsx
@@ -22,46 +22,46 @@
     <t>Mummidi</t>
   </si>
   <si>
-    <t>Shyam</t>
-  </si>
-  <si>
-    <t>Pydi</t>
-  </si>
-  <si>
     <t>shyam@gmail.com</t>
   </si>
   <si>
-    <t>Chaitanya</t>
-  </si>
-  <si>
-    <t>Revu</t>
-  </si>
-  <si>
-    <t>Mohan</t>
-  </si>
-  <si>
-    <t>roa</t>
-  </si>
-  <si>
     <t>Road no:8A</t>
   </si>
   <si>
-    <t>Hyderabad</t>
-  </si>
-  <si>
-    <t>telangana</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
-    <t>Vamsi</t>
-  </si>
-  <si>
-    <t>pogari</t>
-  </si>
-  <si>
     <t>March</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Sydney</t>
+  </si>
+  <si>
+    <t>New South Wales</t>
+  </si>
+  <si>
+    <t>Siddarth</t>
+  </si>
+  <si>
+    <t>Sai</t>
+  </si>
+  <si>
+    <t>saimanoj@yahoo.com</t>
+  </si>
+  <si>
+    <t>February</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>oxford street</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>North east</t>
   </si>
 </sst>
 </file>
@@ -409,26 +409,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="16.54296875" customWidth="1"/>
     <col min="2" max="2" width="17.36328125" customWidth="1"/>
-    <col min="3" max="3" width="18.08984375" customWidth="1"/>
+    <col min="3" max="3" width="19.6328125" customWidth="1"/>
     <col min="4" max="4" width="16.54296875" style="2" customWidth="1"/>
     <col min="5" max="5" width="17.6328125" customWidth="1"/>
     <col min="6" max="6" width="15.90625" customWidth="1"/>
     <col min="7" max="7" width="17.90625" customWidth="1"/>
     <col min="8" max="8" width="19.90625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="13.26953125" customWidth="1"/>
+    <col min="9" max="9" width="15.90625" customWidth="1"/>
     <col min="10" max="10" width="13.54296875" style="2" customWidth="1"/>
     <col min="11" max="11" width="18" customWidth="1"/>
-    <col min="12" max="12" width="8.7265625" style="2"/>
+    <col min="12" max="12" width="10.81640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -438,73 +438,81 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2">
+        <v>1234567898</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="2">
+        <v>500089</v>
+      </c>
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="2">
+        <v>2</v>
+      </c>
+      <c r="K1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="2">
+        <v>2020</v>
+      </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2">
+        <v>9182820148</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="2">
+        <v>530041</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="2">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="2">
-        <v>9182820148</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="K2" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="2">
-        <v>500089</v>
-      </c>
-      <c r="I4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" s="2">
-        <v>2</v>
-      </c>
-      <c r="K5" t="s">
-        <v>15</v>
-      </c>
-      <c r="L5" s="2">
-        <v>2020</v>
+      <c r="L2" s="2">
+        <v>1999</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C1" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>